<commit_message>
added in a bar graph section
</commit_message>
<xml_diff>
--- a/Income by Education Level.xlsx
+++ b/Income by Education Level.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafa_\Desktop\GitHub\Proj3-Team3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicafernandez/Desktop/Proj3-Team3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46683AD7-B71F-4E3E-8077-A480024C3FC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{690EB559-3A22-BA42-B923-B73E6E625AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="0" windowWidth="43680" windowHeight="11820" xr2:uid="{10F3F418-39B5-49F1-8168-998EEB464A5D}"/>
+    <workbookView xWindow="-20" yWindow="3060" windowWidth="28800" windowHeight="17040" xr2:uid="{10F3F418-39B5-49F1-8168-998EEB464A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,9 +506,13 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -530,7 +534,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -541,7 +545,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -552,7 +556,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -563,7 +567,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -574,7 +578,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -585,7 +589,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -596,7 +600,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -607,7 +611,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>